<commit_message>
update actions value real/previ
</commit_message>
<xml_diff>
--- a/php/files/export_temps.xlsx
+++ b/php/files/export_temps.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -68,34 +68,46 @@
     <t>personne</t>
   </si>
   <si>
-    <t>0311948c-1d97-424c-9e65-25d1ef642df2</t>
-  </si>
-  <si>
-    <t>ftg</t>
-  </si>
-  <si>
-    <t>2023-01-05 07:30:00</t>
-  </si>
-  <si>
-    <t>2023-01-05 09:30:00</t>
+    <t>zzzz</t>
+  </si>
+  <si>
+    <t>'2022-04-25 08:30:00</t>
+  </si>
+  <si>
+    <t>'2022-04-25 12:00:00</t>
+  </si>
+  <si>
+    <t>ANIM_TRANSVERSALE</t>
+  </si>
+  <si>
+    <t>PRAM 2022</t>
   </si>
   <si>
     <t>Bureau</t>
   </si>
   <si>
-    <t>blabla</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
-    <t>2023-01-05</t>
-  </si>
-  <si>
-    <t>#3a5a6a</t>
+    <t>'2022-04-29</t>
+  </si>
+  <si>
+    <t>#139410</t>
   </si>
   <si>
     <t>Benoit Perceval</t>
+  </si>
+  <si>
+    <t>ZH PRAM</t>
+  </si>
+  <si>
+    <t>'2022-09-19 12:00:00</t>
+  </si>
+  <si>
+    <t>'2022-09-19 16:30:00</t>
+  </si>
+  <si>
+    <t>'2022-09-19</t>
   </si>
 </sst>
 </file>
@@ -431,7 +443,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,35 +505,37 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>31785</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+      <c r="F2">
+        <v>273</v>
+      </c>
+      <c r="G2">
+        <v>1667</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>455</v>
-      </c>
-      <c r="G2">
-        <v>51615</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2"/>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
       <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
         <v>22</v>
       </c>
+      <c r="K2"/>
       <c r="L2" t="s">
         <v>23</v>
       </c>
@@ -538,6 +552,57 @@
         <v>25</v>
       </c>
       <c r="Q2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>40228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>4.5</v>
+      </c>
+      <c r="F3">
+        <v>273</v>
+      </c>
+      <c r="G3">
+        <v>1667</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>